<commit_message>
chamada e aula02 LOP
</commit_message>
<xml_diff>
--- a/ds/turmas/1DES_A/frequencia-2-A.xlsx
+++ b/ds/turmas/1DES_A/frequencia-2-A.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn1057928\Desktop\senai2026\ds\turmas\1DES_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8844FE3C-B659-4845-BED8-A17FE3690FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6AF738-C8BD-4948-98ED-25D7E7BB90B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,29 +16,17 @@
     <sheet name="chamada" sheetId="1" r:id="rId1"/>
     <sheet name="alunos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
   <si>
     <t>Aluno</t>
   </si>
@@ -225,17 +213,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -528,7 +506,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,8 +526,12 @@
       <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -651,6 +633,33 @@
       <c r="E2" s="1">
         <v>46051</v>
       </c>
+      <c r="F2" s="1">
+        <v>46055</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
@@ -711,6 +720,9 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>33</v>
       </c>
       <c r="AU3" s="2"/>
@@ -807,6 +819,9 @@
       <c r="E4" t="s">
         <v>33</v>
       </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
       <c r="AU4" s="2"/>
       <c r="AV4" s="2"/>
       <c r="AW4" s="2"/>
@@ -901,6 +916,9 @@
       <c r="E5" t="s">
         <v>33</v>
       </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
       <c r="AU5" s="2"/>
       <c r="AV5" s="2"/>
       <c r="AW5" s="2"/>
@@ -995,6 +1013,9 @@
       <c r="E6" t="s">
         <v>33</v>
       </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
       <c r="AU6" s="2"/>
       <c r="AV6" s="2"/>
       <c r="AW6" s="2"/>
@@ -1089,6 +1110,9 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
       <c r="AU7" s="2"/>
       <c r="AV7" s="2"/>
       <c r="AW7" s="2"/>
@@ -1183,6 +1207,9 @@
       <c r="E8" t="s">
         <v>33</v>
       </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
       <c r="AU8" s="2"/>
       <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
@@ -1277,6 +1304,9 @@
       <c r="E9" t="s">
         <v>33</v>
       </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
       <c r="AU9" s="2"/>
       <c r="AV9" s="2"/>
       <c r="AW9" s="2"/>
@@ -1371,6 +1401,9 @@
       <c r="E10" t="s">
         <v>33</v>
       </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
       <c r="AU10" s="2"/>
       <c r="AV10" s="2"/>
       <c r="AW10" s="2"/>
@@ -1465,6 +1498,9 @@
       <c r="E11" t="s">
         <v>33</v>
       </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
       <c r="AU11" s="2"/>
       <c r="AV11" s="2"/>
       <c r="AW11" s="2"/>
@@ -1559,6 +1595,9 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
       <c r="AU12" s="2"/>
       <c r="AV12" s="2"/>
       <c r="AW12" s="2"/>
@@ -1653,6 +1692,9 @@
       <c r="E13" t="s">
         <v>33</v>
       </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
       <c r="AU13" s="2"/>
       <c r="AV13" s="2"/>
       <c r="AW13" s="2"/>
@@ -1747,6 +1789,9 @@
       <c r="E14" t="s">
         <v>33</v>
       </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
       <c r="AU14" s="2"/>
       <c r="AV14" s="2"/>
       <c r="AW14" s="2"/>
@@ -1841,6 +1886,9 @@
       <c r="E15" t="s">
         <v>33</v>
       </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
       <c r="AU15" s="2"/>
       <c r="AV15" s="2"/>
       <c r="AW15" s="2"/>
@@ -1935,6 +1983,9 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
       <c r="AU16" s="2"/>
       <c r="AV16" s="2"/>
       <c r="AW16" s="2"/>
@@ -2029,6 +2080,9 @@
       <c r="E17" t="s">
         <v>33</v>
       </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
       <c r="AU17" s="2"/>
       <c r="AV17" s="2"/>
       <c r="AW17" s="2"/>
@@ -2123,6 +2177,9 @@
       <c r="E18" t="s">
         <v>33</v>
       </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
       <c r="AU18" s="2"/>
       <c r="AV18" s="2"/>
       <c r="AW18" s="2"/>
@@ -2217,6 +2274,9 @@
       <c r="E19" t="s">
         <v>33</v>
       </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
       <c r="AU19" s="2"/>
       <c r="AV19" s="2"/>
       <c r="AW19" s="2"/>
@@ -2311,6 +2371,9 @@
       <c r="E20" t="s">
         <v>33</v>
       </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
       <c r="AU20" s="2"/>
       <c r="AV20" s="2"/>
       <c r="AW20" s="2"/>
@@ -2405,6 +2468,9 @@
       <c r="E21" t="s">
         <v>33</v>
       </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
       <c r="AU21" s="2"/>
       <c r="AV21" s="2"/>
       <c r="AW21" s="2"/>
@@ -2499,6 +2565,9 @@
       <c r="E22" t="s">
         <v>33</v>
       </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
       <c r="AU22" s="2"/>
       <c r="AV22" s="2"/>
       <c r="AW22" s="2"/>
@@ -2593,6 +2662,9 @@
       <c r="E23" t="s">
         <v>33</v>
       </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
       <c r="AU23" s="2"/>
       <c r="AV23" s="2"/>
       <c r="AW23" s="2"/>
@@ -2685,7 +2757,10 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
       </c>
       <c r="AU24" s="2"/>
       <c r="AV24" s="2"/>
@@ -2779,7 +2854,10 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
       </c>
       <c r="AU25" s="2"/>
       <c r="AV25" s="2"/>
@@ -2875,6 +2953,9 @@
       <c r="E26" t="s">
         <v>33</v>
       </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
       <c r="AU26" s="2"/>
       <c r="AV26" s="2"/>
       <c r="AW26" s="2"/>
@@ -2969,6 +3050,9 @@
       <c r="E27" t="s">
         <v>33</v>
       </c>
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
       <c r="AU27" s="2"/>
       <c r="AV27" s="2"/>
       <c r="AW27" s="2"/>
@@ -3063,6 +3147,9 @@
       <c r="E28" t="s">
         <v>33</v>
       </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
       <c r="AU28" s="2"/>
       <c r="AV28" s="2"/>
       <c r="AW28" s="2"/>
@@ -3157,6 +3244,9 @@
       <c r="E29" t="s">
         <v>33</v>
       </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
       <c r="AU29" s="2"/>
       <c r="AV29" s="2"/>
       <c r="AW29" s="2"/>
@@ -3251,6 +3341,9 @@
       <c r="E30" t="s">
         <v>33</v>
       </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
       <c r="AU30" s="2"/>
       <c r="AV30" s="2"/>
       <c r="AW30" s="2"/>
@@ -3345,6 +3438,9 @@
       <c r="E31" t="s">
         <v>33</v>
       </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
       <c r="AU31" s="2"/>
       <c r="AV31" s="2"/>
       <c r="AW31" s="2"/>
@@ -3439,6 +3535,9 @@
       <c r="E32" t="s">
         <v>33</v>
       </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
       <c r="AU32" s="2"/>
       <c r="AV32" s="2"/>
       <c r="AW32" s="2"/>
@@ -3520,7 +3619,7 @@
     <sortCondition ref="B3:B32"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="BE3:DG3 D3:AZ3 BB3:BB22 BE4:BJ10 BK4:DG32 F11:BA22 BC11:BJ22 F23:BJ23 F4:AZ10 D4:E23 D24:BJ32">
+  <conditionalFormatting sqref="D3:AZ3 BE3:DG3 BB3:BB22 F4:AZ10 BE4:BJ10 D4:E23 BK4:DG32 F11:BA22 BC11:BJ22 F23:BJ23 D24:BJ32">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>

</xml_diff>